<commit_message>
Separate US between "Ruahatu - Services" and "Ruahatu - Client".
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$I$34</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="106">
   <si>
     <t>User story</t>
   </si>
@@ -353,6 +353,27 @@
   </si>
   <si>
     <t>48000</t>
+  </si>
+  <si>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>Ruahatu - Services</t>
+  </si>
+  <si>
+    <t>Ruahatu - Client</t>
+  </si>
+  <si>
+    <t>URL REST de suppression des données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sécuriser les URL REST de suppression des données </t>
+  </si>
+  <si>
+    <t>Les inforamtions d'un utilisateur ne peuvent êtresupprimé que par lui ou un administrateur.</t>
+  </si>
+  <si>
+    <t>Ruahatu</t>
   </si>
 </sst>
 </file>
@@ -797,846 +818,1032 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="32.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="14" customWidth="1"/>
-    <col min="5" max="6" width="60.42578125" style="4" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="32.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="14" customWidth="1"/>
+    <col min="6" max="7" width="60.42578125" style="4" customWidth="1"/>
+    <col min="8" max="9" width="12.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="210.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="210.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14">
+      <c r="E3" s="14">
         <v>47000</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14">
+      <c r="E4" s="14">
         <v>46000</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14">
+      <c r="E5" s="14">
         <v>45000</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="14">
+      <c r="E6" s="14">
         <v>44000</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14">
+      <c r="E7" s="14">
         <v>43000</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="14">
+      <c r="E8" s="14">
         <v>42000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="14">
+      <c r="E9" s="14">
         <v>41000</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="14">
+      <c r="E10" s="14">
         <v>40000</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="14">
+      <c r="E11" s="14">
         <v>39000</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="14">
+      <c r="E12" s="14">
         <v>38000</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="14">
+      <c r="E13" s="14">
         <v>37000</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14">
+      <c r="E14" s="14">
         <v>36000</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="14">
+      <c r="E15" s="14">
         <v>35000</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="14">
+      <c r="E16" s="14">
         <v>34000</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="14">
+      <c r="E17" s="14">
         <v>33000</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="14">
+      <c r="E18" s="14">
         <v>32000</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="14">
+      <c r="E19" s="14">
         <v>31000</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="14">
+      <c r="E20" s="14">
         <v>30000</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="14">
+      <c r="E21" s="14">
         <v>29000</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="14">
+      <c r="E22" s="14">
         <v>28000</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="14">
+      <c r="E23" s="14">
         <v>27000</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="14">
+      <c r="E24" s="14">
         <v>26000</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="14">
+      <c r="E25" s="14">
         <v>25000</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="14">
+      <c r="E26" s="14">
         <v>24000</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="14">
+      <c r="E27" s="14">
         <v>23000</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="14">
+      <c r="E28" s="14">
         <v>22000</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="14">
+      <c r="E29" s="14">
         <v>21000</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="14">
+      <c r="E30" s="14">
         <v>20000</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="14">
+      <c r="E31" s="14">
         <v>19000</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
+        <v>49</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="14">
+        <v>18600</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>50</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="14">
+        <v>18300</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
         <v>31</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="14">
-        <v>18000</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
-        <v>32</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="14">
-        <v>17000</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="14">
-        <v>16000</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="14">
+        <v>18000</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="14">
-        <v>15000</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="C35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="14">
+        <v>17000</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="14">
-        <v>14000</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C36" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="14">
+        <v>16000</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="14">
+        <v>15000</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>35</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="14">
+        <v>14000</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>36</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="14">
+      <c r="E39" s="14">
         <v>13000</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
         <v>37</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="14">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
-        <v>38</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="14">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
-        <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="14">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="14">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" s="14">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="14">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="14">
-        <v>8000</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="14">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" s="14">
-        <v>7000</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C43" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="14">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="14">
-        <v>6000</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="14">
+        <v>8000</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="14">
+        <v>7000</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>43</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="14">
+        <v>6000</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>44</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="14">
+      <c r="E47" s="14">
         <v>5000</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C48" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="14">
+      <c r="E48" s="14">
         <v>4000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C49" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="14">
+      <c r="E49" s="14">
         <v>3000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C50" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="14">
+      <c r="E50" s="14">
         <v>2000</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C51" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D49" s="14">
+      <c r="E51" s="14">
         <v>1000</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H32"/>
+  <autoFilter ref="A1:I34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add state and date informations on US.
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="109">
   <si>
     <t>User story</t>
   </si>
@@ -352,9 +352,6 @@
     <t>Suppression d’une famille de poissons</t>
   </si>
   <si>
-    <t>48000</t>
-  </si>
-  <si>
     <t>Projet</t>
   </si>
   <si>
@@ -374,6 +371,18 @@
   </si>
   <si>
     <t>Ruahatu</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>CHECKOUT</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>XX/XX/2010</t>
   </si>
 </sst>
 </file>
@@ -480,7 +489,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -514,6 +523,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,18 +830,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="32.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="8" customWidth="1"/>
     <col min="4" max="4" width="59.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="14" customWidth="1"/>
-    <col min="6" max="7" width="60.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10" style="14" customWidth="1"/>
+    <col min="6" max="6" width="63.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="30" style="4" customWidth="1"/>
     <col min="8" max="9" width="12.5703125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -844,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
@@ -873,16 +884,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>98</v>
+      <c r="E2" s="14">
+        <v>48000</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -893,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>9</v>
@@ -903,6 +920,12 @@
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -913,7 +936,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>11</v>
@@ -923,6 +946,12 @@
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -933,7 +962,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>13</v>
@@ -946,6 +975,12 @@
       </c>
       <c r="G5" s="9" t="s">
         <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -956,7 +991,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>17</v>
@@ -966,6 +1001,12 @@
       </c>
       <c r="F6" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="15">
+        <v>40557</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -976,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>19</v>
@@ -986,6 +1027,12 @@
       </c>
       <c r="F7" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -996,13 +1043,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="14">
         <v>42000</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1013,7 +1066,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>22</v>
@@ -1023,6 +1076,12 @@
       </c>
       <c r="F9" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1033,7 +1092,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>25</v>
@@ -1043,6 +1102,9 @@
       </c>
       <c r="F10" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1053,7 +1115,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>31</v>
@@ -1063,6 +1125,9 @@
       </c>
       <c r="F11" s="4" t="s">
         <v>42</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1073,7 +1138,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>33</v>
@@ -1083,6 +1148,9 @@
       </c>
       <c r="F12" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1093,7 +1161,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>34</v>
@@ -1103,6 +1171,9 @@
       </c>
       <c r="F13" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1113,7 +1184,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>35</v>
@@ -1123,6 +1194,9 @@
       </c>
       <c r="F14" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1133,7 +1207,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>36</v>
@@ -1143,6 +1217,9 @@
       </c>
       <c r="F15" s="4" t="s">
         <v>43</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1153,7 +1230,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>37</v>
@@ -1164,8 +1241,11 @@
       <c r="F16" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1173,7 +1253,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>38</v>
@@ -1184,8 +1264,11 @@
       <c r="F17" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1193,7 +1276,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>44</v>
@@ -1204,8 +1287,11 @@
       <c r="F18" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1213,7 +1299,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>45</v>
@@ -1224,8 +1310,11 @@
       <c r="F19" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1233,7 +1322,7 @@
         <v>48</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>49</v>
@@ -1244,8 +1333,11 @@
       <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1253,7 +1345,7 @@
         <v>48</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>51</v>
@@ -1264,8 +1356,11 @@
       <c r="F21" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1273,7 +1368,7 @@
         <v>48</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>52</v>
@@ -1284,8 +1379,11 @@
       <c r="F22" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1293,7 +1391,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>53</v>
@@ -1304,8 +1402,11 @@
       <c r="F23" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -1313,7 +1414,7 @@
         <v>54</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>55</v>
@@ -1324,8 +1425,11 @@
       <c r="F24" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -1333,7 +1437,7 @@
         <v>54</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>56</v>
@@ -1344,8 +1448,11 @@
       <c r="F25" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -1353,7 +1460,7 @@
         <v>54</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>57</v>
@@ -1364,8 +1471,11 @@
       <c r="F26" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -1373,7 +1483,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>58</v>
@@ -1384,8 +1494,11 @@
       <c r="F27" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -1393,7 +1506,7 @@
         <v>54</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>60</v>
@@ -1404,8 +1517,11 @@
       <c r="F28" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -1413,7 +1529,7 @@
         <v>54</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>61</v>
@@ -1424,8 +1540,11 @@
       <c r="F29" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -1433,7 +1552,7 @@
         <v>65</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>62</v>
@@ -1444,8 +1563,11 @@
       <c r="F30" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -1453,7 +1575,7 @@
         <v>65</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>63</v>
@@ -1464,8 +1586,11 @@
       <c r="F31" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>49</v>
       </c>
@@ -1473,17 +1598,20 @@
         <v>28</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E32" s="14">
         <v>18600</v>
       </c>
       <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H32" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>50</v>
       </c>
@@ -1491,19 +1619,22 @@
         <v>29</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E33" s="14">
         <v>18300</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>31</v>
       </c>
@@ -1511,7 +1642,7 @@
         <v>75</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>66</v>
@@ -1522,8 +1653,11 @@
       <c r="F34" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="H34" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>32</v>
       </c>
@@ -1531,7 +1665,7 @@
         <v>75</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>97</v>
@@ -1542,8 +1676,11 @@
       <c r="F35" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="H35" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>33</v>
       </c>
@@ -1551,7 +1688,7 @@
         <v>75</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>67</v>
@@ -1562,8 +1699,11 @@
       <c r="F36" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="H36" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>34</v>
       </c>
@@ -1571,7 +1711,7 @@
         <v>75</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>68</v>
@@ -1582,8 +1722,11 @@
       <c r="F37" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="H37" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>35</v>
       </c>
@@ -1591,7 +1734,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>69</v>
@@ -1602,8 +1745,11 @@
       <c r="F38" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>36</v>
       </c>
@@ -1611,7 +1757,7 @@
         <v>75</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>70</v>
@@ -1622,8 +1768,11 @@
       <c r="F39" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>37</v>
       </c>
@@ -1631,7 +1780,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>81</v>
@@ -1639,8 +1788,11 @@
       <c r="E40" s="14">
         <v>12000</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>38</v>
       </c>
@@ -1648,7 +1800,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>82</v>
@@ -1656,8 +1808,11 @@
       <c r="E41" s="14">
         <v>11000</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H41" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>39</v>
       </c>
@@ -1665,7 +1820,7 @@
         <v>76</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>77</v>
@@ -1673,8 +1828,11 @@
       <c r="E42" s="14">
         <v>10000</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>40</v>
       </c>
@@ -1682,7 +1840,7 @@
         <v>76</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>78</v>
@@ -1690,8 +1848,11 @@
       <c r="E43" s="14">
         <v>9000</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H43" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>41</v>
       </c>
@@ -1699,7 +1860,7 @@
         <v>76</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>88</v>
@@ -1710,8 +1871,11 @@
       <c r="F44" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>42</v>
       </c>
@@ -1719,7 +1883,7 @@
         <v>76</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>87</v>
@@ -1730,8 +1894,11 @@
       <c r="F45" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>43</v>
       </c>
@@ -1739,7 +1906,7 @@
         <v>76</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>86</v>
@@ -1750,8 +1917,11 @@
       <c r="F46" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>44</v>
       </c>
@@ -1759,7 +1929,7 @@
         <v>76</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>84</v>
@@ -1770,8 +1940,11 @@
       <c r="F47" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>45</v>
       </c>
@@ -1779,7 +1952,7 @@
         <v>90</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>89</v>
@@ -1787,8 +1960,14 @@
       <c r="E48" s="14">
         <v>4000</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>46</v>
       </c>
@@ -1796,7 +1975,7 @@
         <v>29</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>91</v>
@@ -1804,8 +1983,14 @@
       <c r="E49" s="14">
         <v>3000</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>47</v>
       </c>
@@ -1813,7 +1998,7 @@
         <v>54</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>92</v>
@@ -1821,8 +2006,11 @@
       <c r="E50" s="14">
         <v>2000</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H50" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>48</v>
       </c>
@@ -1830,7 +2018,7 @@
         <v>95</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>93</v>
@@ -1840,6 +2028,9 @@
       </c>
       <c r="F51" s="4" t="s">
         <v>94</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DONE US. ruahatu.fr and ruahatu.com buyed.
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="110">
   <si>
     <t>User story</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>XX/XX/2010</t>
+  </si>
+  <si>
+    <t>ruahatu.fr et ruahatu.com achetés.</t>
   </si>
 </sst>
 </file>
@@ -830,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,7 +1878,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>42</v>
       </c>
@@ -1894,8 +1897,11 @@
       <c r="F45" s="9" t="s">
         <v>80</v>
       </c>
+      <c r="G45" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="H45" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add bugs and DONE US.
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$I$34</definedName>
@@ -17,10 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="110">
-  <si>
-    <t>User story</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="119">
   <si>
     <t>State</t>
   </si>
@@ -387,11 +385,44 @@
   <si>
     <t>ruahatu.fr et ruahatu.com achetés.</t>
   </si>
+  <si>
+    <t>Date saisie</t>
+  </si>
+  <si>
+    <t>Numéro</t>
+  </si>
+  <si>
+    <t>Titre</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>User story/Tâches technique</t>
+  </si>
+  <si>
+    <t>Maven</t>
+  </si>
+  <si>
+    <t>Utiliser le module maven</t>
+  </si>
+  <si>
+    <t>Services Web pas assez respectueux des principes REST</t>
+  </si>
+  <si>
+    <t>Affichage - Liste poissons pas assez testé (Selenium)</t>
+  </si>
+  <si>
+    <t>Authentification pas assez testé</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,7 +523,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -527,6 +558,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,16 +864,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="17.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="8" customWidth="1"/>
     <col min="4" max="4" width="59.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="14" customWidth="1"/>
@@ -852,31 +885,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="210.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -884,25 +917,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="14">
         <v>48000</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -910,25 +943,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="14">
         <v>47000</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -936,25 +969,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="14">
         <v>46000</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -962,28 +995,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="14">
         <v>45000</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -991,22 +1024,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="14">
         <v>44000</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" s="15">
         <v>40557</v>
@@ -1017,25 +1050,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="14">
         <v>43000</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1043,22 +1076,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="14">
         <v>42000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1066,25 +1099,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="14">
         <v>41000</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1092,22 +1125,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="14">
         <v>40000</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1115,22 +1148,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="14">
         <v>39000</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1138,22 +1171,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="E12" s="14">
         <v>38000</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1161,22 +1194,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="14">
         <v>37000</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1184,22 +1217,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="14">
         <v>36000</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1207,22 +1240,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="14">
         <v>35000</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1230,22 +1263,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="14">
         <v>34000</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1253,22 +1286,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="14">
         <v>33000</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1276,22 +1309,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="14">
         <v>32000</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1299,22 +1332,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="14">
         <v>31000</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1322,22 +1355,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="E20" s="14">
         <v>30000</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1345,22 +1378,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="14">
         <v>29000</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1368,22 +1401,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="14">
         <v>28000</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,22 +1424,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="14">
         <v>27000</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1414,22 +1447,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="E24" s="14">
         <v>26000</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1437,22 +1470,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="14">
         <v>25000</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1460,22 +1493,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="14">
         <v>24000</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,22 +1516,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="14">
         <v>23000</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,22 +1539,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="14">
         <v>22000</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1529,22 +1562,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="14">
         <v>21000</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1552,22 +1585,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="14">
         <v>20000</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1575,22 +1608,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E31" s="14">
         <v>19000</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1598,20 +1631,20 @@
         <v>49</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="14">
         <v>18600</v>
       </c>
       <c r="F32" s="9"/>
       <c r="H32" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1619,22 +1652,22 @@
         <v>50</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33" s="14">
         <v>18300</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1642,22 +1675,22 @@
         <v>31</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E34" s="14">
         <v>18000</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1665,22 +1698,22 @@
         <v>32</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E35" s="14">
         <v>17000</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1688,22 +1721,22 @@
         <v>33</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="14">
         <v>16000</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1711,22 +1744,22 @@
         <v>34</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" s="14">
         <v>15000</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1734,22 +1767,22 @@
         <v>35</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E38" s="14">
         <v>14000</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1757,22 +1790,22 @@
         <v>36</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E39" s="14">
         <v>13000</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1780,19 +1813,19 @@
         <v>37</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" s="14">
         <v>12000</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1800,19 +1833,19 @@
         <v>38</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41" s="14">
         <v>11000</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1820,19 +1853,19 @@
         <v>39</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="E42" s="14">
         <v>10000</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1840,19 +1873,19 @@
         <v>40</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" s="14">
         <v>9000</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1860,22 +1893,22 @@
         <v>41</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E44" s="14">
         <v>8000</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1883,25 +1916,25 @@
         <v>42</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E45" s="14">
         <v>7000</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1909,22 +1942,22 @@
         <v>43</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" s="14">
         <v>6000</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1932,22 +1965,22 @@
         <v>44</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E47" s="14">
         <v>5000</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1955,22 +1988,22 @@
         <v>45</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48" s="14">
         <v>4000</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1978,22 +2011,22 @@
         <v>46</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E49" s="14">
         <v>3000</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2001,19 +2034,19 @@
         <v>47</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E50" s="14">
         <v>2000</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2021,22 +2054,39 @@
         <v>48</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E51" s="14">
         <v>1000</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2044,4 +2094,87 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="11.42578125" style="17"/>
+    <col min="3" max="3" width="17.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17">
+        <v>40559</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
+        <v>40559</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>40559</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>